<commit_message>
Tweaked component list again and created PCB file. Also created Teensy layout.
</commit_message>
<xml_diff>
--- a/component_list/list.xlsx
+++ b/component_list/list.xlsx
@@ -84,18 +84,9 @@
     <t>Hope RF RFM98W 433</t>
   </si>
   <si>
-    <t>AnArduino</t>
-  </si>
-  <si>
     <t>Custom</t>
   </si>
   <si>
-    <t>http://www.ebay.co.uk/itm/HopeRF-RFM98W-433Mhz-LoRa-Ultra-Long-Range-Transceiver-SX1278-compatible-/181442620537</t>
-  </si>
-  <si>
-    <t>LoRa 433mhz module. Via ebay. Watch lead times vs hoperf.co.uk. Gnd and CS module</t>
-  </si>
-  <si>
     <t>http://uk.rs-online.com/web/p/motor-driver-ics/7140622/</t>
   </si>
   <si>
@@ -166,6 +157,15 @@
   </si>
   <si>
     <t>Total:</t>
+  </si>
+  <si>
+    <t>HABSupplies</t>
+  </si>
+  <si>
+    <t>LoRa 433mhz module. Gnd and CS module</t>
+  </si>
+  <si>
+    <t>http://ava.upuaut.net/store/index.php?route=product/product&amp;product_id=110</t>
   </si>
 </sst>
 </file>
@@ -175,7 +175,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -229,7 +229,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -518,7 +518,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -540,10 +542,10 @@
         <v>7</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>1</v>
@@ -597,7 +599,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>11</v>
@@ -638,28 +640,28 @@
         <v>2</v>
       </c>
       <c r="C5" s="1">
-        <v>5.73</v>
+        <v>5.99</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="0"/>
-        <v>11.46</v>
+        <v>11.98</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="G5" s="2" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
@@ -675,18 +677,18 @@
         <v>6</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
@@ -699,21 +701,21 @@
         <v>24.59</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
@@ -726,21 +728,21 @@
         <v>0.92</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B9" s="3">
         <v>5</v>
@@ -756,22 +758,22 @@
         <v>6</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C11" s="6">
         <f>SUM(D2:D9)</f>
-        <v>75.47</v>
+        <v>75.990000000000009</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -779,31 +781,31 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1">
         <f>0.2*C11</f>
-        <v>15.094000000000001</v>
+        <v>15.198000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1">
         <v>20</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C17" s="1">
         <f>C11+C13+C15</f>
-        <v>110.56399999999999</v>
+        <v>111.18800000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new stabilising caps to parts list. Also to PCB design. Using SparkFun Libraries.
</commit_message>
<xml_diff>
--- a/component_list/list.xlsx
+++ b/component_list/list.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -166,6 +166,18 @@
   </si>
   <si>
     <t>http://ava.upuaut.net/store/index.php?route=product/product&amp;product_id=110</t>
+  </si>
+  <si>
+    <t>4.7uF ceramic</t>
+  </si>
+  <si>
+    <t>0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage reg input/output caps. </t>
+  </si>
+  <si>
+    <t>http://uk.rs-online.com/web/p/ceramic-multilayer-capacitors/7883045/</t>
   </si>
 </sst>
 </file>
@@ -516,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +607,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D9" si="0">B3*C3</f>
+        <f t="shared" ref="D3:D10" si="0">B3*C3</f>
         <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -767,50 +779,77 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="3">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2.78</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>27.799999999999997</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C13" s="6">
         <f>SUM(D2:D9)</f>
         <v>75.990000000000009</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="1">
-        <f>0.2*C11</f>
-        <v>15.198000000000002</v>
-      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="1">
+        <f>0.2*C13</f>
+        <v>15.198000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C17" s="1">
         <v>20</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="1">
-        <f>C11+C13+C15</f>
+      <c r="C19" s="1">
+        <f>C13+C15+C17</f>
         <v>111.18800000000002</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Decided on using a different motor driver, added boost converter, decided on linear servo for parachute release. Not much PCB design completed.
</commit_message>
<xml_diff>
--- a/component_list/list.xlsx
+++ b/component_list/list.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -39,21 +39,6 @@
     <t>Package</t>
   </si>
   <si>
-    <t>Freescale MPL3115A2</t>
-  </si>
-  <si>
-    <t>http://uk.rs-online.com/web/p/absolute-pressure-sensor-ics/7500841/</t>
-  </si>
-  <si>
-    <t>RS</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>LGA</t>
-  </si>
-  <si>
     <t>Teensy 3.1</t>
   </si>
   <si>
@@ -87,15 +72,6 @@
     <t>Custom</t>
   </si>
   <si>
-    <t>http://uk.rs-online.com/web/p/motor-driver-ics/7140622/</t>
-  </si>
-  <si>
-    <t>L293D</t>
-  </si>
-  <si>
-    <t>16-DIP</t>
-  </si>
-  <si>
     <t>Motor driver - ideally to be paired for easier heat dissipation + redundancy.</t>
   </si>
   <si>
@@ -126,9 +102,6 @@
     <t>https://www.sparkfun.com/products/10361</t>
   </si>
   <si>
-    <t>http://uk.rs-online.com/web/p/low-dropout-voltage-regulators/0460522/</t>
-  </si>
-  <si>
     <t>Ultra LDO reg</t>
   </si>
   <si>
@@ -174,10 +147,64 @@
     <t>0805</t>
   </si>
   <si>
-    <t xml:space="preserve">Voltage reg input/output caps. </t>
-  </si>
-  <si>
-    <t>http://uk.rs-online.com/web/p/ceramic-multilayer-capacitors/7883045/</t>
+    <t>Farnell</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/measurement-specialties/ms563702ba03-50/sensor-barometric-0-01-1-2bar-qfn/dp/2362663?Ntt=ms5637</t>
+  </si>
+  <si>
+    <t>MS5637</t>
+  </si>
+  <si>
+    <t>QFN</t>
+  </si>
+  <si>
+    <t>A3901</t>
+  </si>
+  <si>
+    <t>DFN-10</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/allegro-microsystems/a3901sejtr-t/motor-driv-full-bridge-400ma-dfn/dp/1651947</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/texas-instruments/lp2989im-3-3-nopb/ic-linear-voltage-regulator/dp/1652324</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/murata/grm219r6ya475ma73d/cap-mlcc-x5r-4-7uf-35v-0805/dp/2426962?in_merch=New%20Products&amp;in_merch=Featured%20New%20Products&amp;MER=i-9b10-00002068</t>
+  </si>
+  <si>
+    <t>Quantity to be used in CanSat</t>
+  </si>
+  <si>
+    <t>Voltage reg input/output caps. X5R as specified.</t>
+  </si>
+  <si>
+    <t>TPS63061DSCR</t>
+  </si>
+  <si>
+    <t>10-SON</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/texas-instruments/tps63061dscr/buck-boost-5v-2a-10son/dp/2082429</t>
+  </si>
+  <si>
+    <t>Motor power boost - configurable buck/boost converter.</t>
+  </si>
+  <si>
+    <t>SloughRC</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Tiny 2g linear servo motor. Self contained motor control. 3.2-4.2V</t>
+  </si>
+  <si>
+    <t>http://www.sloughrc.com/default.asp?WPG=SRCM_HomePage1&amp;PageNumber=1&amp;s=c:0,c:070,b:Spektrum,c:070-040</t>
+  </si>
+  <si>
+    <t>Spektrum SPMSH2026L</t>
   </si>
 </sst>
 </file>
@@ -528,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,13 +578,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>1</v>
@@ -566,7 +593,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>2</v>
@@ -574,52 +601,52 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="B2" s="3">
         <v>2</v>
       </c>
       <c r="C2" s="1">
-        <v>2.04</v>
+        <v>1.68</v>
       </c>
       <c r="D2" s="1">
         <f>B2*C2</f>
-        <v>4.08</v>
+        <v>3.36</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D10" si="0">B3*C3</f>
+        <f t="shared" ref="D3:D12" si="0">B3*C3</f>
         <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
@@ -632,21 +659,21 @@
         <v>19.059999999999999</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
@@ -659,48 +686,48 @@
         <v>11.98</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
       </c>
       <c r="C6" s="1">
-        <v>3.03</v>
+        <v>0.99</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>6.06</v>
+        <v>1.98</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
@@ -713,21 +740,21 @@
         <v>24.59</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
@@ -740,21 +767,21 @@
         <v>0.92</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B9" s="3">
         <v>5</v>
@@ -767,89 +794,143 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B10" s="3">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1">
         <v>2.78</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>27.799999999999997</v>
+        <v>8.34</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="F10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="6">
-        <f>SUM(D2:D9)</f>
-        <v>75.990000000000009</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2.23</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>2.23</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="1">
-        <f>0.2*C13</f>
-        <v>15.198000000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="1">
+      <c r="F11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>10.49</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>10.49</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="6">
+        <f>SUM(D2:D13)</f>
+        <v>92.25</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="1">
+        <f>0.2*C14</f>
+        <v>18.45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="1">
         <v>20</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="1">
-        <f>C13+C15+C17</f>
-        <v>111.18800000000002</v>
+      <c r="G18" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="1">
+        <f>C14+C16+C18</f>
+        <v>130.69999999999999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Opted for different boost converter and added motors + various other components.
</commit_message>
<xml_diff>
--- a/component_list/list.xlsx
+++ b/component_list/list.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Components" sheetId="1" r:id="rId1"/>
-    <sheet name="PCB manufacture" sheetId="2" r:id="rId2"/>
+    <sheet name="PCB names and values" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
   <si>
     <t>Name</t>
   </si>
@@ -180,18 +180,6 @@
     <t>Voltage reg input/output caps. X5R as specified.</t>
   </si>
   <si>
-    <t>TPS63061DSCR</t>
-  </si>
-  <si>
-    <t>10-SON</t>
-  </si>
-  <si>
-    <t>http://uk.farnell.com/texas-instruments/tps63061dscr/buck-boost-5v-2a-10son/dp/2082429</t>
-  </si>
-  <si>
-    <t>Motor power boost - configurable buck/boost converter.</t>
-  </si>
-  <si>
     <t>SloughRC</t>
   </si>
   <si>
@@ -205,6 +193,78 @@
   </si>
   <si>
     <t>Spektrum SPMSH2026L</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/jst-japan-solderless-terminals/s2b-ph-sm4-tb-lf-sn/connector-header-smt-r-a-2mm-2way/dp/9492615?Ntt=S2B-PH-SM4-TB%28LF%29%28SN</t>
+  </si>
+  <si>
+    <t>JST connector for LiPo</t>
+  </si>
+  <si>
+    <t>JST side entry 2pin 2mm</t>
+  </si>
+  <si>
+    <t>N/A SMD</t>
+  </si>
+  <si>
+    <t>LiPo</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cool Components. From Sparkfun. Self contained discharge protection circuitry </t>
+  </si>
+  <si>
+    <t>https://www.coolcomponents.co.uk/lithium-polymer-battery-2000mah.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Motors</t>
+  </si>
+  <si>
+    <t>eBay - China</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Consider economics of ordering in larger package but paying VAT and handling charge</t>
+  </si>
+  <si>
+    <t>https://www.coolcomponents.co.uk/teensy-3-1.html</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/texas-instruments/lmr62421xmf/boost-1a-24vout/dp/2064678</t>
+  </si>
+  <si>
+    <t>LMR62421XMF</t>
+  </si>
+  <si>
+    <t>SOT-23</t>
+  </si>
+  <si>
+    <t>Boost converter for motors.</t>
+  </si>
+  <si>
+    <t>Component ID</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>JST connector</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>IC1</t>
+  </si>
+  <si>
+    <t>Component</t>
   </si>
 </sst>
 </file>
@@ -555,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +627,7 @@
     <col min="2" max="2" width="28.85546875" style="3" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" style="2" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="2"/>
     <col min="7" max="7" width="78.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="2"/>
@@ -633,15 +693,24 @@
       <c r="B3" s="3">
         <v>2</v>
       </c>
+      <c r="C3" s="1">
+        <v>16.989999999999998</v>
+      </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D12" si="0">B3*C3</f>
-        <v>0</v>
+        <f t="shared" ref="D3:D15" si="0">B3*C3</f>
+        <v>33.979999999999997</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -835,34 +904,34 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="B11" s="3">
         <v>1</v>
       </c>
       <c r="C11" s="1">
-        <v>2.23</v>
+        <v>1.95</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>2.23</v>
+        <v>1.95</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B12" s="3">
         <v>1</v>
@@ -875,62 +944,137 @@
         <v>10.49</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>10.99</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>10.99</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="3">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>3.13</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>6.26</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="6">
-        <f>SUM(D2:D13)</f>
-        <v>92.25</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="C17" s="6">
+        <f>SUM(D2:D15)</f>
+        <v>143.43099999999998</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="1">
-        <f>0.2*C14</f>
-        <v>18.45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="C19" s="1">
+        <f>0.2*C17</f>
+        <v>28.686199999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C21" s="1">
         <v>20</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="1">
-        <f>C14+C16+C18</f>
-        <v>130.69999999999999</v>
+      <c r="C23" s="1">
+        <f>C17+C19+C21</f>
+        <v>192.11719999999997</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E17:G17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -939,12 +1083,54 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="55.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Continued PCB design and added relevant components. Now almost completed boost power supply design.
</commit_message>
<xml_diff>
--- a/component_list/list.xlsx
+++ b/component_list/list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Components" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="96">
   <si>
     <t>Name</t>
   </si>
@@ -60,9 +60,6 @@
     <t>4-SIL</t>
   </si>
   <si>
-    <t>RH humidity &amp; ext air temp - ext mount</t>
-  </si>
-  <si>
     <t>http://www.rapidonline.com/Electronic-Components/IST-AG-HYT-271-Digital-humidity-temperature-sensor-50-9442?sourceRefKey=DsBEy7i-7&amp;filterSearchScope=1</t>
   </si>
   <si>
@@ -183,9 +180,6 @@
     <t>SloughRC</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Tiny 2g linear servo motor. Self contained motor control. 3.2-4.2V</t>
   </si>
   <si>
@@ -265,6 +259,60 @@
   </si>
   <si>
     <t>Component</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>Capacitor for U2</t>
+  </si>
+  <si>
+    <t>4.7uF</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>10nf ceramic</t>
+  </si>
+  <si>
+    <t>10nf</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/avx/0805ya103jat2a/cap-mlcc-c0g-np0-10nf-16v-0805/dp/2332815</t>
+  </si>
+  <si>
+    <t>Voltage reg bypass cap. C0G/NP0 as specified in app notes</t>
+  </si>
+  <si>
+    <t>10K resistors</t>
+  </si>
+  <si>
+    <t>I2C SDA&amp;SCL pullups</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/te-connectivity/crgh0805f10k/resistor-power-10k-0-33w-1-0805/dp/2332084RL</t>
+  </si>
+  <si>
+    <t>rel humidity &amp; ext air temp - ext mount</t>
+  </si>
+  <si>
+    <t>O/B</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>SOD-323</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/nxp/bat760/diode-schottky-sod-323/dp/8734593</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boost power supply diode. 1A forward current. </t>
   </si>
 </sst>
 </file>
@@ -615,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,13 +686,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>1</v>
@@ -661,7 +709,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="3">
         <v>2</v>
@@ -674,16 +722,16 @@
         <v>3.36</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -697,20 +745,20 @@
         <v>16.989999999999998</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D15" si="0">B3*C3</f>
+        <f t="shared" ref="D3:D18" si="0">B3*C3</f>
         <v>33.979999999999997</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -734,15 +782,15 @@
         <v>10</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
@@ -755,21 +803,21 @@
         <v>11.98</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
@@ -782,21 +830,21 @@
         <v>1.98</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
@@ -809,21 +857,21 @@
         <v>24.59</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
@@ -836,21 +884,21 @@
         <v>0.92</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="3">
         <v>5</v>
@@ -863,218 +911,305 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="H9" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.122</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.122</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="3">
-        <v>3</v>
-      </c>
-      <c r="C10" s="1">
-        <v>2.78</v>
-      </c>
-      <c r="D10" s="1">
-        <f t="shared" si="0"/>
-        <v>8.34</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="G10" s="2" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="B11" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11" s="1">
-        <v>1.95</v>
+        <v>2.78</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>1.95</v>
+        <v>8.34</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>55</v>
+      <c r="A12" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="B12" s="3">
         <v>1</v>
       </c>
       <c r="C12" s="1">
-        <v>10.49</v>
+        <v>1.95</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>10.49</v>
+        <v>1.95</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B13" s="3">
         <v>1</v>
       </c>
       <c r="C13" s="1">
-        <v>0.23100000000000001</v>
+        <v>10.49</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>0.23100000000000001</v>
+        <v>10.49</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="H13" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
       </c>
       <c r="C14" s="1">
-        <v>10.99</v>
+        <v>0.23100000000000001</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>10.99</v>
+        <v>0.23100000000000001</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>61</v>
+        <v>39</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>10.99</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>10.99</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3.13</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>6.26</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="3">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="3">
         <v>2</v>
       </c>
-      <c r="C15" s="1">
-        <v>3.13</v>
-      </c>
-      <c r="D15" s="1">
-        <f t="shared" si="0"/>
-        <v>6.26</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="C17" s="1">
+        <v>1.4E-2</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>7.8E-2</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>7.8E-2</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="6">
+        <f>SUM(D2:D18)</f>
+        <v>143.65899999999999</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="6">
-        <f>SUM(D2:D15)</f>
-        <v>143.43099999999998</v>
-      </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="C22" s="1">
+        <f>0.2*C20</f>
+        <v>28.7318</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="1">
-        <f>0.2*C17</f>
-        <v>28.686199999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="C24" s="1">
+        <v>20</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="1">
-        <v>20</v>
-      </c>
-      <c r="G21" s="2" t="s">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="1">
-        <f>C17+C19+C21</f>
-        <v>192.11719999999997</v>
+      <c r="C26" s="1">
+        <f>C20+C22+C24</f>
+        <v>192.39079999999998</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E20:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1083,10 +1218,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1097,26 +1232,26 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -1124,10 +1259,43 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>78</v>
       </c>
-      <c r="B5" t="s">
-        <v>70</v>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished boost power supply and updated component list accordingly.
</commit_message>
<xml_diff>
--- a/component_list/list.xlsx
+++ b/component_list/list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Components" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="127">
   <si>
     <t>Name</t>
   </si>
@@ -291,9 +291,6 @@
     <t>10K resistors</t>
   </si>
   <si>
-    <t>I2C SDA&amp;SCL pullups</t>
-  </si>
-  <si>
     <t>http://uk.farnell.com/te-connectivity/crgh0805f10k/resistor-power-10k-0-33w-1-0805/dp/2332084RL</t>
   </si>
   <si>
@@ -313,6 +310,102 @@
   </si>
   <si>
     <t xml:space="preserve">Boost power supply diode. 1A forward current. </t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>Resistor for IC1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>30.1k</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>Diode for IC1</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>Cap for IC1</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>1nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L1 </t>
+  </si>
+  <si>
+    <t>Inductor for IC1</t>
+  </si>
+  <si>
+    <t>10uH</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/wurth-elektronik/74404042100/inductor-semi-shld-10uh-20-1-2a/dp/2431496</t>
+  </si>
+  <si>
+    <t>Inductor for boost power supply. Semi-shielded. Check stock status before order.</t>
+  </si>
+  <si>
+    <t>I2C SDA&amp;SCL pullups &amp; resistor for boost power supply</t>
+  </si>
+  <si>
+    <t>10uH Inductor</t>
+  </si>
+  <si>
+    <t>10uF ceramic</t>
+  </si>
+  <si>
+    <t>Boost power supply filtering.</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/avx/08053d106kat2a/cap-mlcc-x5r-10uf-25v-0805/dp/1867958RL</t>
+  </si>
+  <si>
+    <t>1nf ceramic</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/avx/08051c102k4z2a/cap-mlcc-x7r-1nf-100v-0805/dp/1833849</t>
+  </si>
+  <si>
+    <t>30K1 resistor</t>
+  </si>
+  <si>
+    <t>Boost power supply</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/vishay-draloric/crcw080530k1fkea/resistor-0805-30k1-1/dp/1652981RL</t>
+  </si>
+  <si>
+    <t>1M resistor</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/multicomp/mc0805s8f1004t5e/resistor-thick-film-1mohm-125mw/dp/1646371</t>
   </si>
 </sst>
 </file>
@@ -324,7 +417,7 @@
     <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,13 +440,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -369,7 +482,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -382,6 +495,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -663,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,7 +861,7 @@
         <v>16.989999999999998</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D18" si="0">B3*C3</f>
+        <f t="shared" ref="D3:D23" si="0">B3*C3</f>
         <v>33.979999999999997</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -782,7 +898,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>11</v>
@@ -1022,7 +1138,7 @@
         <v>50</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>51</v>
@@ -1076,7 +1192,7 @@
         <v>59</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>60</v>
@@ -1103,7 +1219,7 @@
         <v>63</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>65</v>
@@ -1117,14 +1233,14 @@
         <v>87</v>
       </c>
       <c r="B17" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17" s="1">
         <v>1.4E-2</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="0"/>
-        <v>2.8000000000000001E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>39</v>
@@ -1133,15 +1249,15 @@
         <v>38</v>
       </c>
       <c r="G17" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B18" s="3">
         <v>1</v>
@@ -1157,59 +1273,197 @@
         <v>39</v>
       </c>
       <c r="F18" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>94</v>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="6">
-        <f>SUM(D2:D18)</f>
-        <v>143.65899999999999</v>
-      </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
+      <c r="A20" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="3">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>0.76</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>30</v>
+      <c r="A22" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1</v>
       </c>
       <c r="C22" s="1">
-        <f>0.2*C20</f>
-        <v>28.7318</v>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="0"/>
+        <v>2E-3</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="1">
-        <v>20</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="G24" s="9"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="6">
+        <f>SUM(D2:D22)</f>
+        <v>145.37299999999999</v>
+      </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="1">
+        <f>0.2*C26</f>
+        <v>29.0746</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="1">
+        <v>20</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="1">
-        <f>C20+C22+C24</f>
-        <v>192.39079999999998</v>
+      <c r="C32" s="1">
+        <f>C26+C28+C30</f>
+        <v>194.44759999999999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E26:G26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1218,10 +1472,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1242,60 +1496,149 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="10" t="s">
         <v>74</v>
       </c>
+      <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
+      <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B8" s="10" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" t="s">
-        <v>84</v>
+      <c r="C8" s="10"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="10"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added A3901 motor control unit and hooked it up. Only pressure sensor, GPS & possibly SD to go.
</commit_message>
<xml_diff>
--- a/component_list/list.xlsx
+++ b/component_list/list.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="132">
   <si>
     <t>Name</t>
   </si>
@@ -406,6 +406,21 @@
   </si>
   <si>
     <t>http://uk.farnell.com/multicomp/mc0805s8f1004t5e/resistor-thick-film-1mohm-125mw/dp/1646371</t>
+  </si>
+  <si>
+    <t>Boost power supply filtering. Motor controller filtering.</t>
+  </si>
+  <si>
+    <t>IC2</t>
+  </si>
+  <si>
+    <t>Motor driver - A3901</t>
+  </si>
+  <si>
+    <t>Teensy pin 3,4 and 5,6</t>
+  </si>
+  <si>
+    <t>GREEN HIGHLIGHT INDICATES COMPONENT ON ORDER LIST</t>
   </si>
 </sst>
 </file>
@@ -492,12 +507,12 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -782,7 +797,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1302,7 +1317,7 @@
       <c r="F19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H19" s="2" t="s">
@@ -1314,14 +1329,14 @@
         <v>117</v>
       </c>
       <c r="B20" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C20" s="1">
         <v>0.38</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" si="0"/>
-        <v>0.76</v>
+        <v>1.1400000000000001</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>39</v>
@@ -1329,8 +1344,8 @@
       <c r="F20" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="9" t="s">
-        <v>118</v>
+      <c r="G20" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>119</v>
@@ -1356,7 +1371,7 @@
       <c r="F21" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G21" s="8" t="s">
         <v>118</v>
       </c>
       <c r="H21" s="2" t="s">
@@ -1383,7 +1398,7 @@
       <c r="F22" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G22" s="8" t="s">
         <v>123</v>
       </c>
       <c r="H22" s="2" t="s">
@@ -1410,7 +1425,7 @@
       <c r="F23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="G23" s="8" t="s">
         <v>123</v>
       </c>
       <c r="H23" s="2" t="s">
@@ -1418,7 +1433,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G24" s="9"/>
+      <c r="G24" s="8"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
@@ -1426,11 +1441,11 @@
       </c>
       <c r="C26" s="6">
         <f>SUM(D2:D22)</f>
-        <v>145.37299999999999</v>
-      </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
+        <v>145.75299999999999</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
@@ -1438,7 +1453,7 @@
       </c>
       <c r="C28" s="1">
         <f>0.2*C26</f>
-        <v>29.0746</v>
+        <v>29.150599999999997</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1458,7 +1473,7 @@
       </c>
       <c r="C32" s="1">
         <f>C26+C28+C30</f>
-        <v>194.44759999999999</v>
+        <v>194.90359999999998</v>
       </c>
     </row>
   </sheetData>
@@ -1472,19 +1487,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
     <col min="2" max="2" width="55.7109375" customWidth="1"/>
+    <col min="4" max="4" width="74.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>71</v>
       </c>
@@ -1494,151 +1510,171 @@
       <c r="C1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="10"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="C3" s="9"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="10"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="C4" s="9"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="10"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="C8" s="9"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C12" s="10"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="C12" s="9"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added pressure sensor. Updated component list. Ordered a number of components. Teensy now SMD on a few pins to permit RFM98W mounting on other side of board.
</commit_message>
<xml_diff>
--- a/component_list/list.xlsx
+++ b/component_list/list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Components" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="135">
   <si>
     <t>Name</t>
   </si>
@@ -405,9 +405,6 @@
     <t>1M resistor</t>
   </si>
   <si>
-    <t>http://uk.farnell.com/multicomp/mc0805s8f1004t5e/resistor-thick-film-1mohm-125mw/dp/1646371</t>
-  </si>
-  <si>
     <t>Boost power supply filtering. Motor controller filtering.</t>
   </si>
   <si>
@@ -421,6 +418,18 @@
   </si>
   <si>
     <t>GREEN HIGHLIGHT INDICATES COMPONENT ON ORDER LIST</t>
+  </si>
+  <si>
+    <t>100nF ceramic</t>
+  </si>
+  <si>
+    <t>Pressure sensor power smoothing</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/avx/08051c104k4z2a/cap-mlcc-x7r-100nf-100v-0805/dp/1833851</t>
+  </si>
+  <si>
+    <t>http://uk.farnell.com/welwyn/cr0805f-1m0fi/resistor-chip-1m-0-125w-1/dp/2341052</t>
   </si>
 </sst>
 </file>
@@ -470,7 +479,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -480,6 +489,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -497,7 +512,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -507,12 +522,17 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -794,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,30 +858,30 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="11">
         <v>2</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="12">
         <v>1.68</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="12">
         <f>B2*C2</f>
         <v>3.36</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="10" t="s">
         <v>40</v>
       </c>
     </row>
@@ -876,7 +896,7 @@
         <v>16.989999999999998</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D23" si="0">B3*C3</f>
+        <f t="shared" ref="D3:D24" si="0">B3*C3</f>
         <v>33.979999999999997</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -946,30 +966,30 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="11">
         <v>2</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="12">
         <v>0.99</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="12">
         <f t="shared" si="0"/>
         <v>1.98</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="10" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1027,111 +1047,111 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="11">
         <v>5</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="12">
         <v>1.86</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="12">
         <f t="shared" si="0"/>
         <v>9.3000000000000007</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="11">
         <v>1</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="12">
         <v>0.122</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="12">
         <f t="shared" si="0"/>
         <v>0.122</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="10" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="11">
         <v>3</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="12">
         <v>2.78</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="12">
         <f t="shared" si="0"/>
         <v>8.34</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="11">
         <v>1</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="12">
         <v>1.95</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="12">
         <f t="shared" si="0"/>
         <v>1.95</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="10" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1162,30 +1182,30 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="11">
         <v>1</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="12">
         <v>0.23100000000000001</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="12">
         <f t="shared" si="0"/>
         <v>0.23100000000000001</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="10" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1243,242 +1263,269 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="11">
         <v>3</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="12">
         <v>1.4E-2</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="12">
         <f t="shared" si="0"/>
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="10" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="11">
         <v>1</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="12">
         <v>7.8E-2</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="12">
         <f t="shared" si="0"/>
         <v>7.8E-2</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="10" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="11">
         <v>1</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="12">
         <v>0.79200000000000004</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="12">
         <f t="shared" si="0"/>
         <v>0.79200000000000004</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="10" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="11">
         <v>3</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="12">
         <v>0.38</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="12">
         <f t="shared" si="0"/>
         <v>1.1400000000000001</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="H20" s="2" t="s">
+      <c r="G20" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="H20" s="10" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="11">
         <v>1</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="12">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="12">
         <f t="shared" si="0"/>
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="10" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="11">
         <v>1</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="12">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="12">
         <f t="shared" si="0"/>
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" s="10" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+    <row r="23" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="11">
         <v>1</v>
       </c>
-      <c r="C23" s="1">
-        <v>2E-3</v>
-      </c>
-      <c r="D23" s="1">
-        <f t="shared" si="0"/>
-        <v>2E-3</v>
-      </c>
-      <c r="E23" s="2" t="s">
+      <c r="C23" s="12">
+        <v>0.76</v>
+      </c>
+      <c r="D23" s="12">
+        <f t="shared" si="0"/>
+        <v>0.76</v>
+      </c>
+      <c r="E23" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>126</v>
+      <c r="H23" s="10" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G24" s="8"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A24" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="0"/>
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G25" s="7"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="6">
-        <f>SUM(D2:D22)</f>
-        <v>145.75299999999999</v>
-      </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="C27" s="6">
+        <f>SUM(D2:D25)</f>
+        <v>146.71699999999998</v>
+      </c>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="1">
-        <f>0.2*C26</f>
-        <v>29.150599999999997</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="C29" s="1">
+        <f>0.2*C27</f>
+        <v>29.343399999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C31" s="1">
         <v>20</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="1">
-        <f>C26+C28+C30</f>
-        <v>194.90359999999998</v>
+      <c r="C33" s="1">
+        <f>C27+C29+C31</f>
+        <v>196.06039999999999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E27:G27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1489,8 +1536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1516,165 +1563,165 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="9"/>
+      <c r="C3" s="8"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="8"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="9"/>
+      <c r="C8" s="8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C12" s="9"/>
+      <c r="C12" s="8"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="8" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="C17" s="8"/>
+      <c r="D17" t="s">
         <v>129</v>
-      </c>
-      <c r="C17" s="9"/>
-      <c r="D17" t="s">
-        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Further changes to RF section. Now has a ground plane of sorts under the RFM98W. Hopefully this will be sufficient - we'll find out!
</commit_message>
<xml_diff>
--- a/component_list/list.xlsx
+++ b/component_list/list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Components" sheetId="1" r:id="rId1"/>
@@ -524,15 +524,15 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -816,7 +816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
@@ -858,30 +858,30 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="10">
         <v>2</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="11">
         <v>1.68</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="11">
         <f>B2*C2</f>
         <v>3.36</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>40</v>
       </c>
     </row>
@@ -966,30 +966,30 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="10">
         <v>2</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <v>0.99</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="11">
         <f t="shared" si="0"/>
         <v>1.98</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="9" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1047,111 +1047,111 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="10">
         <v>5</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="11">
         <v>1.86</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="11">
         <f t="shared" si="0"/>
         <v>9.3000000000000007</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="10">
         <v>1</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="11">
         <v>0.122</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="11">
         <f t="shared" si="0"/>
         <v>0.122</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="10">
         <v>3</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="11">
         <v>2.78</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="11">
         <f t="shared" si="0"/>
         <v>8.34</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="10">
         <v>1</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="11">
         <v>1.95</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="11">
         <f t="shared" si="0"/>
         <v>1.95</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="9" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1182,30 +1182,30 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+    <row r="14" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="10">
         <v>1</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="11">
         <v>0.23100000000000001</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="11">
         <f t="shared" si="0"/>
         <v>0.23100000000000001</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="9" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1263,192 +1263,192 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+    <row r="17" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="10">
         <v>3</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="11">
         <v>1.4E-2</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="11">
         <f t="shared" si="0"/>
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="9" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+    <row r="18" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="10">
         <v>1</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="11">
         <v>7.8E-2</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="11">
         <f t="shared" si="0"/>
         <v>7.8E-2</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="9" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+    <row r="19" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19" s="10">
         <v>1</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="11">
         <v>0.79200000000000004</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="11">
         <f t="shared" si="0"/>
         <v>0.79200000000000004</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+    <row r="20" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="10">
         <v>3</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="11">
         <v>0.38</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="11">
         <f t="shared" si="0"/>
         <v>1.1400000000000001</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="9" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+    <row r="21" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="10">
         <v>1</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="11">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="11">
         <f t="shared" si="0"/>
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="G21" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="H21" s="9" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+    <row r="22" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="10">
         <v>1</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="11">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="11">
         <f t="shared" si="0"/>
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="15" t="s">
+      <c r="G22" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="H22" s="9" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+    <row r="23" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23" s="10">
         <v>1</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="11">
         <v>0.76</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="11">
         <f t="shared" si="0"/>
         <v>0.76</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G23" s="15" t="s">
+      <c r="G23" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="H23" s="9" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1490,9 +1490,9 @@
         <f>SUM(D2:D25)</f>
         <v>146.71699999999998</v>
       </c>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
@@ -1536,8 +1536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Work on Rev. B
</commit_message>
<xml_diff>
--- a/component_list/list.xlsx
+++ b/component_list/list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Components" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="139">
   <si>
     <t>Name</t>
   </si>
@@ -430,6 +430,18 @@
   </si>
   <si>
     <t>http://uk.farnell.com/welwyn/cr0805f-1m0fi/resistor-chip-1m-0-125w-1/dp/2341052</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>RFM98W</t>
+  </si>
+  <si>
+    <t>IC3</t>
+  </si>
+  <si>
+    <t>Barom</t>
   </si>
 </sst>
 </file>
@@ -816,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1480,6 +1492,9 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="G25" s="7"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1534,10 +1549,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1724,6 +1739,22 @@
         <v>129</v>
       </c>
     </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Completed design of motor driver circuitry. Need to update lists.
</commit_message>
<xml_diff>
--- a/component_list/list.xlsx
+++ b/component_list/list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Components" sheetId="1" r:id="rId1"/>
@@ -828,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,7 +1551,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Revision B. Gerbers exported and component list roughly up to date.
</commit_message>
<xml_diff>
--- a/component_list/list.xlsx
+++ b/component_list/list.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Components" sheetId="1" r:id="rId1"/>
     <sheet name="PCB names and values" sheetId="2" r:id="rId2"/>
+    <sheet name="Audit" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="159">
   <si>
     <t>Name</t>
   </si>
@@ -408,15 +409,6 @@
     <t>Boost power supply filtering. Motor controller filtering.</t>
   </si>
   <si>
-    <t>IC2</t>
-  </si>
-  <si>
-    <t>Motor driver - A3901</t>
-  </si>
-  <si>
-    <t>Teensy pin 3,4 and 5,6</t>
-  </si>
-  <si>
     <t>GREEN HIGHLIGHT INDICATES COMPONENT ON ORDER LIST</t>
   </si>
   <si>
@@ -442,6 +434,75 @@
   </si>
   <si>
     <t>Barom</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>Cap for motor driver</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>Motor driver - DRV8833PWP</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>30k1</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>2.2uF</t>
+  </si>
+  <si>
+    <t>Quantity Remaining</t>
+  </si>
+  <si>
+    <t>More req?</t>
+  </si>
+  <si>
+    <t>IST HYT271</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>NB one new and one remaining from previous project</t>
+  </si>
+  <si>
+    <t>One of questionable value - may be damaged</t>
+  </si>
+  <si>
+    <t>Useless to us now - switching to DRV8833 because easier to solder</t>
+  </si>
+  <si>
+    <t>Boost reg</t>
+  </si>
+  <si>
+    <t>100nf</t>
+  </si>
+  <si>
+    <t>LP2989IM</t>
+  </si>
+  <si>
+    <t>Schottky diode</t>
+  </si>
+  <si>
+    <t>2 on each board - enough for NOW</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>JSTs</t>
+  </si>
+  <si>
+    <t>10nF</t>
   </si>
 </sst>
 </file>
@@ -828,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,12 +1522,12 @@
         <v>123</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B24" s="3">
         <v>1</v>
@@ -1485,10 +1546,10 @@
         <v>38</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1496,6 +1557,11 @@
         <v>83</v>
       </c>
       <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
@@ -1549,10 +1615,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1578,7 +1644,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1727,32 +1793,266 @@
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="C17" s="8"/>
-      <c r="D17" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C21" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>156</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>157</v>
+      </c>
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added servo trace, few new power rail pads; new silkscreen note. Exported gerbers for manufacture.
</commit_message>
<xml_diff>
--- a/component_list/list.xlsx
+++ b/component_list/list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Components" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="161">
   <si>
     <t>Name</t>
   </si>
@@ -503,6 +503,12 @@
   </si>
   <si>
     <t>10nF</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>Servo</t>
   </si>
 </sst>
 </file>
@@ -889,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1615,10 +1621,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1843,6 +1849,17 @@
       </c>
       <c r="C22" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C23" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>